<commit_message>
application.cfc and error mangemnt
</commit_message>
<xml_diff>
--- a/files/result_file.xlsx
+++ b/files/result_file.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t/>
   </si>
@@ -41,43 +41,76 @@
     <t>Result</t>
   </si>
   <si>
-    <t>Devi</t>
+    <t>Anoop</t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>anoopjoy8@gmail.com</t>
+  </si>
+  <si>
+    <t>5/16/94</t>
+  </si>
+  <si>
+    <t>Cleaner,Driver</t>
+  </si>
+  <si>
+    <t>Address missing</t>
+  </si>
+  <si>
+    <t>Arun</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>arun23@sd.in</t>
+  </si>
+  <si>
+    <t>3/6/90</t>
+  </si>
+  <si>
+    <t>Admin,Keeper</t>
+  </si>
+  <si>
+    <t>Last name missing,Keeper is not a valid role</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Addrees line 1</t>
+  </si>
+  <si>
+    <t>adam@yourmail.com</t>
+  </si>
+  <si>
+    <t>8/16/90</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>successfully updated</t>
+  </si>
+  <si>
+    <t>Ram</t>
   </si>
   <si>
     <t>K</t>
   </si>
   <si>
-    <t>devi89@gh.in</t>
-  </si>
-  <si>
-    <t>3/9/94</t>
-  </si>
-  <si>
-    <t>Admin,Cleaner</t>
-  </si>
-  <si>
-    <t>Address missing</t>
-  </si>
-  <si>
-    <t>Raju</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>raj56@23.in</t>
-  </si>
-  <si>
-    <t>2/8/70</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>successfully updated</t>
+    <t>ram@yourdomain.com</t>
+  </si>
+  <si>
+    <t>6/8/91</t>
+  </si>
+  <si>
+    <t>Driver,Cleaner</t>
   </si>
 </sst>
 </file>
@@ -135,20 +168,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="7" max="7" width="14.27734375" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="19.5703125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="21.8515625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="13.91015625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="39.9453125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.80859375" customWidth="true" bestFit="true"/>
     <col min="1" max="1" width="10.95703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.39453125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.390625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.7265625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="7.1953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.3046875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="8.3125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -191,7 +224,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>565655.0</v>
+        <v>8.7832327676E10</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -208,25 +241,77 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="n">
+        <v>9.0456766762E10</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="n">
-        <v>34343.0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9.865451223E9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4.512457889E9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>